<commit_message>
Include Glyphicons in menu.
</commit_message>
<xml_diff>
--- a/templates/stroustrup_toc.xlsx
+++ b/templates/stroustrup_toc.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcallah/GitProjects/OOP/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DDD8E6-8B29-7F4B-9660-D3C30B0A16ED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10840" yWindow="700" windowWidth="34580" windowHeight="25600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10840" yWindow="700" windowWidth="34580" windowHeight="25600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="course_struct.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="572">
   <si>
     <t>Object-Oriented Programming</t>
   </si>
@@ -1732,12 +1731,24 @@
   </si>
   <si>
     <t>20.4 Linked lists</t>
+  </si>
+  <si>
+    <t>glyphicon-home</t>
+  </si>
+  <si>
+    <t>glyphicon-list</t>
+  </si>
+  <si>
+    <t>glyphicon-blackboard</t>
+  </si>
+  <si>
+    <t>glyphicon-info-sign</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2057,11 +2068,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D570"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A362" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
-      <selection activeCell="B383" sqref="B383"/>
+    <sheetView tabSelected="1" topLeftCell="A556" zoomScale="244" zoomScaleNormal="244" zoomScalePageLayoutView="244" workbookViewId="0">
+      <selection activeCell="E570" sqref="E570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2070,9 +2081,10 @@
     <col min="2" max="2" width="48.83203125" customWidth="1"/>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2093,16 +2105,22 @@
       <c r="C3" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2121,7 +2139,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -2145,7 +2163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -2153,7 +2171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>4</v>
       </c>
@@ -2161,7 +2179,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -6383,7 +6401,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="561" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A561" s="1">
         <v>5</v>
       </c>
@@ -6391,7 +6409,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="562" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A562" s="1">
         <v>5</v>
       </c>
@@ -6399,7 +6417,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="563" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A563" s="1">
         <v>5</v>
       </c>
@@ -6407,7 +6425,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="564" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A564" s="1">
         <v>4</v>
       </c>
@@ -6415,15 +6433,18 @@
         <v>462</v>
       </c>
     </row>
-    <row r="566" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A566" s="1">
         <v>1</v>
       </c>
       <c r="B566" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="567" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E566" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A567" s="1">
         <v>2</v>
       </c>
@@ -6434,7 +6455,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="568" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A568" s="1">
         <v>2</v>
       </c>
@@ -6445,7 +6466,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="570" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A570" s="1">
         <v>1</v>
       </c>
@@ -6454,6 +6475,9 @@
       </c>
       <c r="C570" t="s">
         <v>563</v>
+      </c>
+      <c r="E570" t="s">
+        <v>571</v>
       </c>
     </row>
   </sheetData>

</xml_diff>